<commit_message>
in progress regency expats
</commit_message>
<xml_diff>
--- a/Inputs/Orange/benefits.xlsx
+++ b/Inputs/Orange/benefits.xlsx
@@ -25,7 +25,7 @@
     <author> </author>
   </authors>
   <commentList>
-    <comment ref="C25" authorId="0">
+    <comment ref="C24" authorId="0">
       <text>
         <r>
           <rPr>
@@ -49,7 +49,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D25" authorId="0">
+    <comment ref="D24" authorId="0">
       <text>
         <r>
           <rPr>
@@ -73,7 +73,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E25" authorId="0">
+    <comment ref="E24" authorId="0">
       <text>
         <r>
           <rPr>
@@ -97,7 +97,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F25" authorId="0">
+    <comment ref="F24" authorId="0">
       <text>
         <r>
           <rPr>
@@ -121,7 +121,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G25" authorId="0">
+    <comment ref="G24" authorId="0">
       <text>
         <r>
           <rPr>
@@ -150,7 +150,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="110">
   <si>
     <t xml:space="preserve">User Type</t>
   </si>
@@ -206,16 +206,16 @@
     <t xml:space="preserve">Network Details</t>
   </si>
   <si>
-    <t xml:space="preserve">NAS Comprehensive Network</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NAS General Network</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NAS Restricted Network</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NAS Super Restricted Network</t>
+    <t xml:space="preserve">Neuron General Network Plus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Neuron General Network</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Neuron Restricted Network</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Neuron Restricted Network 1</t>
   </si>
   <si>
     <t xml:space="preserve">NAS Workers Network (OP &amp; IP available at Hospitals)</t>
@@ -243,10 +243,7 @@
     <t xml:space="preserve">Chronic Condition Cover</t>
   </si>
   <si>
-    <t xml:space="preserve">Covered in full</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Covered up to AED 250,000</t>
+    <t xml:space="preserve">Covered up to the Annual Maximum Limit(AML) if evidence of continuity of coverage (COC) in UAE is provided; otherwise, the limit will be restricted to AED 150,000 .Treatment for chronic and pre-existing conditions excluded for first 6 months of first scheme membership, included thereafter.This requirement is waived in the event that there is an emergency case where the cover is up to AML.</t>
   </si>
   <si>
     <t xml:space="preserve">Pre-existing Condition Cover</t>
@@ -305,28 +302,16 @@
     <t xml:space="preserve">Organ Transplant</t>
   </si>
   <si>
-    <t xml:space="preserve">Covered up to AED 25,000, subject to pre-apporval
-(recipient only excluding cost organ)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Covered up to AED 10,000, subject to pre-apporval
-(recipient only excluding cost organ)</t>
+    <t xml:space="preserve">Covered up to maximum AED 100,000 with 20% co-pay subject to prior approval</t>
   </si>
   <si>
     <t xml:space="preserve">Out-patient (Consultations, Lab &amp; Diagnostics, Pharmacy, Physiotherapy)</t>
   </si>
   <si>
-    <t xml:space="preserve">Out-patient benefits</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Medicines covered in full with $ co-pay; OP covered in full with $  co-pay
-Consultations covered with $ co-pay</t>
-  </si>
-  <si>
     <t xml:space="preserve">Out-patient Consultations</t>
   </si>
   <si>
-    <t xml:space="preserve">Covered in full with $ co-pay</t>
+    <t xml:space="preserve">Covered in full with  co-pay</t>
   </si>
   <si>
     <t xml:space="preserve">Out-patient Specialists</t>
@@ -335,7 +320,7 @@
     <t xml:space="preserve">Out-patient Medicines</t>
   </si>
   <si>
-    <t xml:space="preserve">Covered in full with $ co-pay
+    <t xml:space="preserve">Covered in full with  co-pay
 (Optional Benefits Available)</t>
   </si>
   <si>
@@ -380,6 +365,9 @@
     <t xml:space="preserve">Complications of Pregnancy</t>
   </si>
   <si>
+    <t xml:space="preserve">Covered in full</t>
+  </si>
+  <si>
     <t xml:space="preserve">New Born Cover</t>
   </si>
   <si>
@@ -498,12 +486,6 @@
   </si>
   <si>
     <t xml:space="preserve">Nil (Pharmacy Co-pay)/5% (Pharmacy Co-pay)/10% (Pharmacy Co-pay)/15% (Pharmacy Co-pay)/20% (Pharmacy Co-pay)/25% (Pharmacy Co-pay)/30% (Pharmacy Co-pay)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nil/Nil/Nil-5%/5%/5%-10%/10%/10%-15%/15%/15%/-20%/20%/20%-25%/25%/25%-30%/30%/30%</t>
   </si>
   <si>
     <t xml:space="preserve">In-patient only</t>
@@ -613,6 +595,13 @@
     </font>
     <font>
       <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -623,12 +612,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF222222"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -704,7 +687,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -769,11 +752,15 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -785,16 +772,16 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -891,20 +878,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H53"/>
+  <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H19" activeCellId="0" sqref="H19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F9" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G21" activeCellId="0" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="60.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="3" style="0" width="59.37"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -930,7 +917,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
@@ -953,7 +940,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="8" t="s">
         <v>14</v>
       </c>
@@ -976,7 +963,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="10" t="s">
         <v>14</v>
       </c>
@@ -1012,7 +999,7 @@
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
     </row>
-    <row r="6" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="13" t="s">
         <v>25</v>
       </c>
@@ -1035,58 +1022,58 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="78.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
         <v>28</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="16" t="s">
         <v>30</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>30</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="78.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
         <v>28</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="16" t="s">
         <v>30</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>30</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
@@ -1094,96 +1081,96 @@
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
     </row>
-    <row r="10" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="46.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="13" t="s">
         <v>28</v>
       </c>
       <c r="B10" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="D10" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="G10" s="17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="E10" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="F10" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="G10" s="16" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="17" t="s">
+      <c r="C11" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="D11" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="E11" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="F11" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="G11" s="18" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D11" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="G11" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
         <v>25</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C12" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="E12" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="F12" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="G12" s="18" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C12" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="F12" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="G12" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
         <v>25</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C13" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="E13" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="F13" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="G13" s="18" t="s">
-        <v>37</v>
+        <v>38</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="F13" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="G13" s="19" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1191,45 +1178,45 @@
         <v>25</v>
       </c>
       <c r="B14" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="D14" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="E14" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="F14" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="G14" s="19" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D14" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="F14" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="G14" s="20" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
         <v>25</v>
       </c>
       <c r="B15" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="D15" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="E15" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="F15" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="G15" s="15" t="s">
-        <v>44</v>
+      <c r="D15" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="F15" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="G15" s="21" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1237,7 +1224,7 @@
         <v>23</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
@@ -1245,27 +1232,27 @@
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
     </row>
-    <row r="17" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="B17" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="C17" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="D17" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="E17" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="F17" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="G17" s="20" t="s">
-        <v>47</v>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1273,71 +1260,71 @@
         <v>25</v>
       </c>
       <c r="B18" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="H18" s="22" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="D19" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="E19" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="F19" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="G19" s="23" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D18" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B19" s="5" t="s">
+      <c r="C20" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="H19" s="21" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="B20" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="C20" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="D20" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="E20" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="F20" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="G20" s="20" t="s">
-        <v>52</v>
+      <c r="D20" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1345,127 +1332,128 @@
         <v>25</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B22" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E22" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C22" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>49</v>
-      </c>
       <c r="F22" s="4" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+    </row>
+    <row r="24" customFormat="false" ht="35.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B23" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C23" s="4" t="s">
+      <c r="B24" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="C24" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="D24" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="E24" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="F24" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="G24" s="15" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="35.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F23" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="G23" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B24" s="12" t="s">
+      <c r="C25" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-    </row>
-    <row r="25" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="B25" s="14" t="s">
+      <c r="D25" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="E25" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="F25" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="G25" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="H25" s="22"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C25" s="15" t="s">
+      <c r="C26" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="D25" s="15" t="s">
+      <c r="D26" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="E25" s="15" t="s">
+      <c r="E26" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F25" s="15" t="s">
+      <c r="F26" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="G25" s="15" t="s">
+      <c r="G26" s="4" t="s">
         <v>62</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C26" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="D26" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="E26" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="F26" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="G26" s="15" t="s">
-        <v>64</v>
       </c>
       <c r="H26" s="22"/>
     </row>
@@ -1474,165 +1462,164 @@
         <v>25</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>30</v>
+        <v>64</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>30</v>
+        <v>64</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>30</v>
+        <v>64</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>30</v>
+        <v>64</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>30</v>
+        <v>64</v>
       </c>
       <c r="H27" s="22"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B28" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C29" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="D29" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="E28" s="4" t="s">
+      <c r="E29" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="F28" s="4" t="s">
+      <c r="F29" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="G28" s="4" t="s">
+      <c r="G29" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="H28" s="22"/>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B29" s="12" t="s">
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B30" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="B30" s="14" t="s">
+      <c r="C30" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C30" s="20" t="s">
+      <c r="D30" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="F30" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="D30" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="E30" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="F30" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="G30" s="13" t="s">
+      <c r="G30" s="4" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B31" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="1"/>
+    </row>
+    <row r="32" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B31" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="C31" s="4" t="s">
+      <c r="B32" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="D31" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="G31" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B32" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-      <c r="G32" s="1"/>
+      <c r="C32" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="D32" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="E32" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="F32" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="G32" s="13" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B33" s="23" t="s">
+      <c r="B33" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C33" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="D33" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="E33" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="F33" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="G33" s="20" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B34" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="C33" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="D33" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="E33" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="F33" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="G33" s="13" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B34" s="5" t="s">
+      <c r="C34" s="25" t="s">
         <v>76</v>
       </c>
-      <c r="C34" s="19" t="s">
+      <c r="D34" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="D34" s="19" t="s">
-        <v>77</v>
-      </c>
-      <c r="E34" s="19" t="s">
-        <v>77</v>
-      </c>
-      <c r="F34" s="19" t="s">
-        <v>77</v>
-      </c>
-      <c r="G34" s="19" t="s">
-        <v>77</v>
+      <c r="E34" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="F34" s="25" t="s">
+        <v>79</v>
+      </c>
+      <c r="G34" s="25" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1640,114 +1627,114 @@
         <v>25</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C35" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="D35" s="24" t="s">
-        <v>80</v>
-      </c>
-      <c r="E35" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="F35" s="24" t="s">
+      <c r="C35" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="G35" s="24" t="s">
+      <c r="D35" s="4" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E35" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="4" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="E36" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="F36" s="4" t="s">
+      <c r="C36" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="G36" s="4" t="s">
+      <c r="D36" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="E36" s="25" t="s">
         <v>89</v>
+      </c>
+      <c r="F36" s="25" t="s">
+        <v>90</v>
+      </c>
+      <c r="G36" s="25" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="C37" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="D37" s="24" t="s">
-        <v>91</v>
-      </c>
-      <c r="E37" s="24" t="s">
+      <c r="C37" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="F37" s="24" t="s">
-        <v>93</v>
-      </c>
-      <c r="G37" s="24" t="s">
-        <v>93</v>
+      <c r="D37" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="B38" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="C38" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="C38" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="E38" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="F38" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="G38" s="4" t="s">
-        <v>95</v>
+      <c r="D38" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="E38" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="F38" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="G38" s="20" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B39" s="25" t="s">
-        <v>96</v>
-      </c>
-      <c r="C39" s="19" t="s">
-        <v>97</v>
-      </c>
-      <c r="D39" s="19" t="s">
-        <v>97</v>
-      </c>
-      <c r="E39" s="19" t="s">
-        <v>97</v>
-      </c>
-      <c r="F39" s="19" t="s">
-        <v>97</v>
-      </c>
-      <c r="G39" s="19" t="s">
-        <v>97</v>
+      <c r="B39" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="G39" s="4" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1755,81 +1742,81 @@
         <v>25</v>
       </c>
       <c r="B40" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="G40" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B41" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="C41" s="4"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="4"/>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B42" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="C40" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="E40" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="F40" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="G40" s="4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="D41" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="E41" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="F41" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="G41" s="4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B42" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="C42" s="4"/>
-      <c r="D42" s="4"/>
-      <c r="E42" s="4"/>
-      <c r="F42" s="4"/>
-      <c r="G42" s="4"/>
+      <c r="C42" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G42" s="4" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="4" t="s">
         <v>28</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1837,235 +1824,189 @@
         <v>28</v>
       </c>
       <c r="B44" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G44" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="35.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B45" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="C45" s="23" t="s">
         <v>102</v>
       </c>
-      <c r="C44" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="D44" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="E44" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="F44" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="G44" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="D45" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="E45" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="F45" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="G45" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D45" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="E45" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="F45" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="G45" s="23" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B46" s="10" t="s">
+      <c r="B46" s="27" t="s">
+        <v>103</v>
+      </c>
+      <c r="C46" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="C46" s="20" t="s">
-        <v>105</v>
-      </c>
-      <c r="D46" s="20" t="s">
-        <v>105</v>
-      </c>
-      <c r="E46" s="20" t="s">
-        <v>105</v>
-      </c>
-      <c r="F46" s="20" t="s">
-        <v>105</v>
-      </c>
-      <c r="G46" s="20" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="31.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D46" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="F46" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="G46" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B47" s="26" t="s">
-        <v>106</v>
-      </c>
-      <c r="C47" s="16" t="s">
-        <v>107</v>
-      </c>
-      <c r="D47" s="16" t="s">
-        <v>107</v>
-      </c>
-      <c r="E47" s="16" t="s">
-        <v>107</v>
-      </c>
-      <c r="F47" s="16" t="s">
-        <v>107</v>
-      </c>
-      <c r="G47" s="16" t="s">
-        <v>107</v>
+      <c r="B47" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="F47" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="G47" s="4" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B48" s="26" t="s">
-        <v>108</v>
+      <c r="B48" s="27" t="s">
+        <v>107</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="G48" s="4" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B49" s="26" t="s">
-        <v>110</v>
+      <c r="B49" s="27" t="s">
+        <v>66</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="G49" s="4" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B50" s="26" t="s">
-        <v>112</v>
+      <c r="B50" s="27" t="s">
+        <v>108</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="G50" s="4" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B51" s="26" t="s">
-        <v>69</v>
+      <c r="B51" s="27" t="s">
+        <v>109</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="G51" s="4" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B52" s="26" t="s">
-        <v>113</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="D52" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="E52" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="F52" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="G52" s="4" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B53" s="26" t="s">
-        <v>114</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="D53" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="E53" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="F53" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="G53" s="4" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
orange plans in progress
</commit_message>
<xml_diff>
--- a/Inputs/Orange/benefits.xlsx
+++ b/Inputs/Orange/benefits.xlsx
@@ -206,16 +206,16 @@
     <t xml:space="preserve">Network Details</t>
   </si>
   <si>
-    <t xml:space="preserve">Neuron General Network Plus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Neuron General Network</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Neuron Restricted Network</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Neuron Restricted Network 1</t>
+    <t xml:space="preserve">NAS Comprehensive Network</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NAS General Network</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NAS Restricted Network</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NAS Super Restricted Network</t>
   </si>
   <si>
     <t xml:space="preserve">NAS Workers Network (OP &amp; IP available at Hospitals)</t>
@@ -586,18 +586,18 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <b val="true"/>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
@@ -732,11 +732,11 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -752,7 +752,7 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -772,7 +772,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -880,11 +880,11 @@
   </sheetPr>
   <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F9" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G21" activeCellId="0" sqref="G21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="40" zoomScaleNormal="40" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="60.99"/>

</xml_diff>